<commit_message>
feat: completed Study Advisor Step 1–3 setup (Supabase storage, auth, uploads, credits, regeneration) + Step 3.10 UX polish and URL cleanup
- Step 1: Created Supabase storage buckets (SOP PDFs, templates, etc.)
- Step 2: Configured storage policies, RLS, and Supabase client
- Step 3: Integrated app with Supabase (auth, upload, download)
- Added database tracking (sop_files) and RLS policies
- Implemented credits system (add/use via RPC)
- Added regeneration flow (consume credit → generate PDF → upload → refresh)
- Step 3.10: Added UX polish (disabled buttons, colored status toasts)
- Sanitized app.html, finder.html, and test.html (removed real Supabase URLs)
- Verified .gitignore excludes .env.local and sensitive files
</commit_message>
<xml_diff>
--- a/universities.xlsx
+++ b/universities.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanthinturi/Desktop/Study Advisor/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7AC4E2-C4F4-C74F-8574-1B6E93ED6FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -187,8 +193,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,13 +270,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +322,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -342,6 +356,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -376,9 +391,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -551,14 +567,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -598,7 +614,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -618,7 +634,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -638,7 +654,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -658,7 +674,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -678,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -698,7 +714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -718,7 +734,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -738,7 +754,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -758,7 +774,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -780,16 +796,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Privacy Policy and Terms of Service: added email, governing law, termination clause, and clarified change notice
</commit_message>
<xml_diff>
--- a/universities.xlsx
+++ b/universities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanthinturi/Desktop/Study Advisor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7AC4E2-C4F4-C74F-8574-1B6E93ED6FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF86332-FEF6-D749-A4D0-204CD2CD4D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,7 +570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>